<commit_message>
added the page of todo show all in detail.
</commit_message>
<xml_diff>
--- a/portfolio03/01/requirement_definition/page_transition/portfolio03_01_pages.xlsx
+++ b/portfolio03/01/requirement_definition/page_transition/portfolio03_01_pages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\programfile\portforio03\01\requirement_definition\page_transition\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Programming\portfolio\portfolio03\01\requirement_definition\page_transition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22E44971-AA05-442E-9568-F68CCC390440}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78C39C0-E291-4E9D-8D29-1F7EF173D66D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{44D0DD1E-12B2-4897-A376-7BC49D58CE45}"/>
+    <workbookView xWindow="5115" yWindow="420" windowWidth="15375" windowHeight="10635" xr2:uid="{44D0DD1E-12B2-4897-A376-7BC49D58CE45}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1"/>
@@ -222,16 +222,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>管理者ログイン機能</t>
-    <rPh sb="0" eb="3">
-      <t>カンリシャ</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>キノウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>ToDo全表示機能</t>
     <rPh sb="4" eb="5">
       <t>ゼン</t>
@@ -280,6 +270,29 @@
     </rPh>
     <rPh sb="7" eb="9">
       <t>ガメン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ToDo詳細表示画面</t>
+    <rPh sb="4" eb="6">
+      <t>ショウサイ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ガメン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>管理者ログイン・ログアウト機能</t>
+    <rPh sb="0" eb="3">
+      <t>カンリシャ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>キノウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -678,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DE1AC94-53EA-4A34-A916-043B2DFA3102}">
-  <dimension ref="B2:E13"/>
+  <dimension ref="B2:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -742,7 +755,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>16</v>
@@ -784,7 +797,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>18</v>
@@ -826,7 +839,7 @@
         <v>7</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>20</v>
@@ -843,7 +856,7 @@
         <v>13</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.4">
@@ -857,7 +870,21 @@
         <v>15</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B14" s="1">
+        <v>12</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>